<commit_message>
lodge achieve rework and char badges
</commit_message>
<xml_diff>
--- a/SSX3/offsetmath.xlsx
+++ b/SSX3/offsetmath.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="195">
   <si>
     <t>Mem</t>
   </si>
@@ -249,9 +249,6 @@
     <t>32bit Mac Longest Rail (decimal left 2 places)</t>
   </si>
   <si>
-    <t>32bit Mac Logest Air Time</t>
-  </si>
-  <si>
     <t>[Bit Flags] Mac Completion Flags</t>
   </si>
   <si>
@@ -595,6 +592,15 @@
   </si>
   <si>
     <t>Offset Hex</t>
+  </si>
+  <si>
+    <t>4aa96c</t>
+  </si>
+  <si>
+    <t>32bit Mac Longest Air Time</t>
+  </si>
+  <si>
+    <t>32bit Mac Most Points</t>
   </si>
 </sst>
 </file>
@@ -934,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L122" sqref="L122"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="Q69" sqref="Q69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,21 +965,21 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" t="s">
         <v>191</v>
-      </c>
-      <c r="H2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -989,7 +995,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1005,7 +1011,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1021,7 +1027,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1037,7 +1043,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1053,7 +1059,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1069,7 +1075,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1085,7 +1091,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1101,7 +1107,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1117,7 +1123,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1133,7 +1139,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1149,7 +1155,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1165,7 +1171,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1181,7 +1187,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1197,7 +1203,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1213,7 +1219,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1229,7 +1235,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1245,7 +1251,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1261,7 +1267,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1277,7 +1283,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1293,7 +1299,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1309,7 +1315,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1381,7 +1387,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1397,7 +1403,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1413,7 +1419,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1429,7 +1435,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1445,7 +1451,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1461,7 +1467,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1477,7 +1483,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1493,7 +1499,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1509,7 +1515,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1525,7 +1531,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1541,7 +1547,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1557,7 +1563,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1573,7 +1579,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1589,7 +1595,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1605,7 +1611,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1621,7 +1627,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1693,7 +1699,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -1709,7 +1715,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -1781,7 +1787,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
@@ -1797,7 +1803,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
         <v>53</v>
@@ -1813,7 +1819,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
         <v>54</v>
@@ -1829,7 +1835,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
         <v>55</v>
@@ -1845,7 +1851,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s">
         <v>56</v>
@@ -1861,7 +1867,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
         <v>57</v>
@@ -1877,7 +1883,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B61" t="s">
         <v>58</v>
@@ -1893,7 +1899,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B62" t="s">
         <v>59</v>
@@ -1909,7 +1915,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B63" t="s">
         <v>60</v>
@@ -1925,7 +1931,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B64" t="s">
         <v>61</v>
@@ -1941,7 +1947,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
         <v>62</v>
@@ -1957,7 +1963,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" t="s">
         <v>63</v>
@@ -1973,7 +1979,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B67" t="s">
         <v>64</v>
@@ -1989,7 +1995,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B68" t="s">
         <v>65</v>
@@ -2005,7 +2011,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B69" t="s">
         <v>66</v>
@@ -2015,13 +2021,13 @@
         <v>3040</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" ref="H69:H124" si="2">DEC2HEX(G69)</f>
+        <f t="shared" ref="H69:H125" si="2">DEC2HEX(G69)</f>
         <v>BE0</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B70" t="s">
         <v>67</v>
@@ -2037,13 +2043,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B71" t="s">
         <v>68</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" ref="G71:G124" si="3">HEX2DEC(A71)-HEX2DEC($A$2)</f>
+        <f t="shared" ref="G71:G125" si="3">HEX2DEC(A71)-HEX2DEC($A$2)</f>
         <v>3042</v>
       </c>
       <c r="H71" t="str">
@@ -2053,7 +2059,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B72" t="s">
         <v>69</v>
@@ -2069,7 +2075,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B73" t="s">
         <v>67</v>
@@ -2085,7 +2091,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
         <v>70</v>
@@ -2101,7 +2107,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B75" t="s">
         <v>71</v>
@@ -2117,7 +2123,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
         <v>72</v>
@@ -2133,7 +2139,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
         <v>73</v>
@@ -2149,7 +2155,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B78" t="s">
         <v>74</v>
@@ -2165,7 +2171,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B79" t="s">
         <v>75</v>
@@ -2181,7 +2187,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B80" t="s">
         <v>76</v>
@@ -2197,10 +2203,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="G81" s="1">
         <f t="shared" si="3"/>
@@ -2213,38 +2219,40 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="G82" s="1">
         <f t="shared" si="3"/>
+        <v>3628</v>
+      </c>
+      <c r="H82" t="str">
+        <f t="shared" si="2"/>
+        <v>E2C</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" t="s">
+        <v>77</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="3"/>
         <v>3880</v>
       </c>
-      <c r="H82" t="str">
+      <c r="H83" t="str">
         <f t="shared" si="2"/>
         <v>F28</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" t="s">
-        <v>79</v>
-      </c>
-      <c r="G83" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H83" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G84" s="1">
         <f t="shared" si="3"/>
@@ -2258,7 +2266,7 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G85" s="1">
         <f t="shared" si="3"/>
@@ -2272,7 +2280,7 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G86" s="1">
         <f t="shared" si="3"/>
@@ -2284,39 +2292,39 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>185</v>
-      </c>
+      <c r="A87" s="1"/>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G87" s="1">
         <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H87" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B88" t="s">
+        <v>77</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="3"/>
         <v>3881</v>
       </c>
-      <c r="H87" t="str">
+      <c r="H88" t="str">
         <f t="shared" si="2"/>
         <v>F29</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" t="s">
-        <v>83</v>
-      </c>
-      <c r="G88" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H88" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G89" s="1">
         <f t="shared" si="3"/>
@@ -2330,7 +2338,7 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G90" s="1">
         <f t="shared" si="3"/>
@@ -2344,7 +2352,7 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G91" s="1">
         <f t="shared" si="3"/>
@@ -2358,7 +2366,7 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G92" s="1">
         <f t="shared" si="3"/>
@@ -2370,39 +2378,39 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="A93" s="1"/>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G93" s="1">
         <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" t="s">
+        <v>77</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" si="3"/>
         <v>3882</v>
       </c>
-      <c r="H93" t="str">
+      <c r="H94" t="str">
         <f t="shared" si="2"/>
         <v>F2A</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" t="s">
-        <v>88</v>
-      </c>
-      <c r="G94" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H94" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G95" s="1">
         <f t="shared" si="3"/>
@@ -2416,7 +2424,7 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G96" s="1">
         <f t="shared" si="3"/>
@@ -2430,7 +2438,7 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G97" s="1">
         <f t="shared" si="3"/>
@@ -2444,7 +2452,7 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G98" s="1">
         <f t="shared" si="3"/>
@@ -2458,81 +2466,81 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" t="s">
+        <v>91</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H99" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" t="s">
+        <v>92</v>
+      </c>
+      <c r="G100" s="1">
+        <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H100" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B101" t="s">
+        <v>77</v>
+      </c>
+      <c r="G101" s="1">
+        <f t="shared" si="3"/>
+        <v>3883</v>
+      </c>
+      <c r="H101" t="str">
+        <f t="shared" si="2"/>
+        <v>F2B</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" t="s">
         <v>93</v>
       </c>
-      <c r="G99" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H99" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+      <c r="G102" s="1">
+        <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H102" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B100" t="s">
-        <v>78</v>
-      </c>
-      <c r="G100" s="1">
-        <f t="shared" si="3"/>
-        <v>3883</v>
-      </c>
-      <c r="H100" t="str">
-        <f t="shared" si="2"/>
-        <v>F2B</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
-      <c r="B101" t="s">
+      <c r="B103" t="s">
         <v>94</v>
       </c>
-      <c r="G101" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H101" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B102" t="s">
-        <v>95</v>
-      </c>
-      <c r="G102" s="1">
+      <c r="G103" s="1">
         <f t="shared" si="3"/>
         <v>3927</v>
       </c>
-      <c r="H102" t="str">
+      <c r="H103" t="str">
         <f t="shared" si="2"/>
         <v>F57</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
-      <c r="B103" t="s">
-        <v>96</v>
-      </c>
-      <c r="G103" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H103" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G104" s="1">
         <f t="shared" si="3"/>
@@ -2546,7 +2554,7 @@
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G105" s="1">
         <f t="shared" si="3"/>
@@ -2560,7 +2568,7 @@
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G106" s="1">
         <f t="shared" si="3"/>
@@ -2574,7 +2582,7 @@
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G107" s="1">
         <f t="shared" si="3"/>
@@ -2588,7 +2596,7 @@
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G108" s="1">
         <f t="shared" si="3"/>
@@ -2602,7 +2610,7 @@
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G109" s="1">
         <f t="shared" si="3"/>
@@ -2616,7 +2624,7 @@
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G110" s="1">
         <f t="shared" si="3"/>
@@ -2628,39 +2636,39 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="A111" s="1"/>
       <c r="B111" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G111" s="1">
         <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H111" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" t="s">
+        <v>94</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" si="3"/>
         <v>3928</v>
       </c>
-      <c r="H111" t="str">
+      <c r="H112" t="str">
         <f t="shared" si="2"/>
         <v>F58</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="1"/>
-      <c r="B112" t="s">
-        <v>104</v>
-      </c>
-      <c r="G112" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H112" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G113" s="1">
         <f t="shared" si="3"/>
@@ -2674,7 +2682,7 @@
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G114" s="1">
         <f t="shared" si="3"/>
@@ -2688,7 +2696,7 @@
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G115" s="1">
         <f t="shared" si="3"/>
@@ -2702,7 +2710,7 @@
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G116" s="1">
         <f t="shared" si="3"/>
@@ -2716,7 +2724,7 @@
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G117" s="1">
         <f t="shared" si="3"/>
@@ -2730,7 +2738,7 @@
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G118" s="1">
         <f t="shared" si="3"/>
@@ -2744,7 +2752,7 @@
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G119" s="1">
         <f t="shared" si="3"/>
@@ -2756,39 +2764,39 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="A120" s="1"/>
       <c r="B120" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="G120" s="1">
         <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H120" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B121" t="s">
+        <v>94</v>
+      </c>
+      <c r="G121" s="1">
+        <f t="shared" si="3"/>
         <v>3929</v>
       </c>
-      <c r="H120" t="str">
+      <c r="H121" t="str">
         <f t="shared" si="2"/>
         <v>F59</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A121" s="1"/>
-      <c r="B121" t="s">
-        <v>112</v>
-      </c>
-      <c r="G121" s="1">
-        <f t="shared" si="3"/>
-        <v>-4889408</v>
-      </c>
-      <c r="H121" t="str">
-        <f t="shared" si="2"/>
-        <v>FFFFB564C0</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G122" s="1">
         <f t="shared" si="3"/>
@@ -2802,7 +2810,7 @@
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G123" s="1">
         <f t="shared" si="3"/>
@@ -2816,13 +2824,27 @@
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G124" s="1">
         <f t="shared" si="3"/>
         <v>-4889408</v>
       </c>
       <c r="H124" t="str">
+        <f t="shared" si="2"/>
+        <v>FFFFB564C0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" t="s">
+        <v>114</v>
+      </c>
+      <c r="G125" s="1">
+        <f t="shared" si="3"/>
+        <v>-4889408</v>
+      </c>
+      <c r="H125" t="str">
         <f t="shared" si="2"/>
         <v>FFFFB564C0</v>
       </c>

</xml_diff>